<commit_message>
canopy cover generate module implemented
</commit_message>
<xml_diff>
--- a/backend/generated/Monster Trial - Corpus Christi/cc_boundary/cc_boundary_20240109_rgb_cc_alfalfa_mosaic.xlsx
+++ b/backend/generated/Monster Trial - Corpus Christi/cc_boundary/cc_boundary_20240109_rgb_cc_alfalfa_mosaic.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,11 +464,6 @@
           <t>20240109</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>geometry</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -493,12 +488,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56133406427764 27.77870440826625, -97.56127165831194 27.7787046789096, -97.56127155936052 27.778686628428048, -97.5613339653159 27.77868635778435, -97.56133406427764 27.77870440826625)))</t>
-        </is>
+        <v>36.15187382156221</v>
       </c>
     </row>
     <row r="3">
@@ -524,12 +514,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56126339578101 27.778705460809594, -97.5612009898161 27.778705731420995, -97.56120089087634 27.778687680939825, -97.56126329683097 27.778687410328093, -97.56126339578101 27.778705460809594)))</t>
-        </is>
+        <v>43.18512393755113</v>
       </c>
     </row>
     <row r="4">
@@ -555,12 +540,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56118540616592 27.778705052923105, -97.56112300020268 27.77870532349927, -97.56112290127582 27.778687273018555, -97.56118530722877 27.77868700244202, -97.56118540616592 27.778705052923105)))</t>
-        </is>
+        <v>14.17988118938711</v>
       </c>
     </row>
     <row r="5">
@@ -586,12 +566,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.5611118381606 27.778705371892038, -97.56104943219859 27.77870564243496, -97.56104933328388 27.778687591954636, -97.56111173923559 27.77868732141136, -97.5611118381606 27.778705371892038)))</t>
-        </is>
+        <v>14.46408889828333</v>
       </c>
     </row>
     <row r="6">
@@ -617,12 +592,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56103674806008 27.77870569741991, -97.56097434209931 27.778705967928904, -97.560974243197 27.778687917449, -97.56103664914745 27.77868764693966, -97.56103674806008 27.77870569741991)))</t>
-        </is>
+        <v>6.229167795332166</v>
       </c>
     </row>
     <row r="7">
@@ -648,12 +618,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56096318005766 27.778706016309656, -97.56090077409812 27.778706286785408, -97.56090067520796 27.778688236305907, -97.5609630811572 27.778687965829807, -97.56096318005766 27.778706016309656)))</t>
-        </is>
+        <v>12.04594757992816</v>
       </c>
     </row>
     <row r="8">
@@ -679,12 +644,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56133391542183 27.77867350792684, -97.56127151249683 27.778674117625798, -97.56127128957509 27.778656068018567, -97.56133369248977 27.778655458319303, -97.56133391542183 27.77867350792684)))</t>
-        </is>
+        <v>23.8212848256756</v>
       </c>
     </row>
     <row r="9">
@@ -710,12 +670,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56126061539211 27.778675185859626, -97.56119821246735 27.77867579552543, -97.56119798955774 27.778657745918533, -97.56126039247219 27.77865713625244, -97.56126061539211 27.778675185859626)))</t>
-        </is>
+        <v>38.26068594584124</v>
       </c>
     </row>
     <row r="10">
@@ -741,12 +696,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56118551171475 27.778675075338406, -97.56112310879124 27.778675684970274, -97.56112288589402 27.778657635363725, -97.56118528880724 27.778657025731583, -97.56118551171475 27.778675075338406)))</t>
-        </is>
+        <v>21.43054609577148</v>
       </c>
     </row>
     <row r="11">
@@ -772,12 +722,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56111296197446 27.778675784094744, -97.5610505590517 27.778676393693782, -97.56105033616647 27.778658344087592, -97.56111273907894 27.778657734488235, -97.56111296197446 27.778675784094744)))</t>
-        </is>
+        <v>36.85519139964804</v>
       </c>
     </row>
     <row r="12">
@@ -803,12 +748,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56103944002997 27.778676774092208, -97.56097703710779 27.77867738365801, -97.56097681423472 27.778659334052154, -97.56103921714657 27.778658724486053, -97.56103944002997 27.778676774092208)))</t>
-        </is>
+        <v>42.17963890126777</v>
       </c>
     </row>
     <row r="13">
@@ -834,12 +774,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56096419435809 27.778676794306236, -97.56090179143713 27.77867740383803, -97.5609015685765 27.778659354232516, -97.56096397148715 27.778658744700422, -97.56096419435809 27.778676794306236)))</t>
-        </is>
+        <v>33.0578973668903</v>
       </c>
     </row>
     <row r="14">
@@ -865,12 +800,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56133383611522 27.778627799676215, -97.56127143120374 27.778628215632384, -97.56127127912106 27.778610165442906, -97.56133368402224 27.778609749486417, -97.56133383611522 27.778627799676215)))</t>
-        </is>
+        <v>46.37618400860777</v>
       </c>
     </row>
     <row r="15">
@@ -896,12 +826,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56126026934975 27.778628290028077, -97.56119786443928 27.778628705950986, -97.56119771236877 27.77861065576189, -97.56126011726892 27.778610239838656, -97.56126026934975 27.778628290028077)))</t>
-        </is>
+        <v>36.20023636075</v>
       </c>
     </row>
     <row r="16">
@@ -927,12 +852,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56118568787149 27.778628787103383, -97.5611232829621 27.778629202992587, -97.56112313090388 27.77861115280387, -97.561185535803 27.778610736914352, -97.56118568787149 27.778628787103383)))</t>
-        </is>
+        <v>49.49106929131641</v>
       </c>
     </row>
     <row r="17">
@@ -958,12 +878,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.5611111139973 27.77863018664785, -97.56104870908841 27.778630602503316, -97.56104855704253 27.778612552314996, -97.56111096194113 27.778612136459202, -97.5611111139973 27.77863018664785)))</t>
-        </is>
+        <v>34.55137010425472</v>
       </c>
     </row>
     <row r="18">
@@ -989,12 +904,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56103602516392 27.778630687023337, -97.56097362025606 27.778631102844876, -97.56097346822261 27.77861305265694, -97.56103587312016 27.778612636835074, -97.56103602516392 27.778630687023337)))</t>
-        </is>
+        <v>22.92929907279351</v>
       </c>
     </row>
     <row r="19">
@@ -1020,12 +930,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56096346551509 27.778630267946077, -97.56090106060874 27.778630683734832, -97.56090090858729 27.778612633547258, -97.56096331348328 27.778612217758194, -97.56096346551509 27.778630267946077)))</t>
-        </is>
+        <v>31.02294172764158</v>
       </c>
     </row>
     <row r="20">
@@ -1051,12 +956,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56133565885219 27.77859717791454, -97.56127325395813 27.77859759387218, -97.561273101875 27.778579543682625, -97.56133550675871 27.77857912772466, -97.56133565885219 27.77859717791454)))</t>
-        </is>
+        <v>35.08699557419547</v>
       </c>
     </row>
     <row r="21">
@@ -1082,12 +982,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.5612623878908 27.778598614785604, -97.56119998299728 27.778599030710126, -97.56119983092621 27.778580980520935, -97.56126223580944 27.77858056459611, -97.5612623878908 27.778598614785604)))</t>
-        </is>
+        <v>52.43948124387937</v>
       </c>
     </row>
     <row r="22">
@@ -1113,12 +1008,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56118651087858 27.778599607924352, -97.56112410598581 27.77860002381454, -97.56112395392732 27.77858197362577, -97.56118635880976 27.77858155773523, -97.56118651087858 27.778599607924352)))</t>
-        </is>
+        <v>49.38161259357787</v>
       </c>
     </row>
     <row r="23">
@@ -1144,12 +1034,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56111379612112 27.778599742234242, -97.56105139122955 27.77860015809159, -97.56105123918309 27.778582107903162, -97.5611136440643 27.778581692045513, -97.56111379612112 27.778599742234242)))</t>
-        </is>
+        <v>31.02058455188471</v>
       </c>
     </row>
     <row r="24">
@@ -1175,12 +1060,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56103851594399 27.778599832465254, -97.56097611105372 27.778600248288573, -97.56097595901966 27.778582198100548, -97.56103836389963 27.778581782276905, -97.56103851594399 27.778599832465254)))</t>
-        </is>
+        <v>45.64289133893747</v>
       </c>
     </row>
     <row r="25">
@@ -1206,12 +1086,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56096445032178 27.77859985758662, -97.5609020454328 27.778600273376476, -97.56090189341099 27.778582223188824, -97.56096429828963 27.77858180739864, -97.56096445032178 27.77859985758662)))</t>
-        </is>
+        <v>34.7198460975232</v>
       </c>
     </row>
     <row r="26">
@@ -1237,12 +1112,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56133522618644 27.778552556809, -97.5612728197247 27.77855268214304, -97.56127277390344 27.778534631492537, -97.56133518035486 27.778534506158135, -97.56133522618644 27.778552556809)))</t>
-        </is>
+        <v>35.36163876974017</v>
       </c>
     </row>
     <row r="27">
@@ -1268,12 +1138,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56126022553995 27.778552689648237, -97.56119781907967 27.778552814948377, -97.56119777327078 27.77853476429833, -97.56126017972073 27.77853463899782, -97.56126022553995 27.778552689648237)))</t>
-        </is>
+        <v>42.49935911110952</v>
       </c>
     </row>
     <row r="28">
@@ -1299,12 +1164,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56118707426297 27.778552854303978, -97.56112466780412 27.77855297957107, -97.5611246220073 27.778534928921456, -97.56118702845588 27.77853480365399, -97.56118707426297 27.778552854303978)))</t>
-        </is>
+        <v>45.43875343077235</v>
       </c>
     </row>
     <row r="29">
@@ -1330,12 +1190,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56111277902137 27.77855287962217, -97.56105037256398 27.7785530048557, -97.56105032677944 27.778534954206524, -97.56111273322651 27.778534828972624, -97.56111277902137 27.77855287962217)))</t>
-        </is>
+        <v>28.45211111649501</v>
       </c>
     </row>
     <row r="30">
@@ -1361,12 +1216,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56103910025963 27.778554573659505, -97.56097669380279 27.778554698859715, -97.56097664803043 27.778536648210974, -97.56103905447698 27.77853652301038, -97.56103910025963 27.778554573659505)))</t>
-        </is>
+        <v>40.31644222904758</v>
       </c>
     </row>
     <row r="31">
@@ -1392,12 +1242,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56095954946983 27.778553117702504, -97.56089714301544 27.778553242866806, -97.5608970972562 27.778535192218524, -97.56095950370027 27.778535067053863, -97.56095954946983 27.778553117702504)))</t>
-        </is>
+        <v>33.15774574200091</v>
       </c>
     </row>
     <row r="32">
@@ -1423,12 +1268,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56133509248168 27.778521532079314, -97.56127268615536 27.778521366786148, -97.5612727465972 27.77850331616962, -97.56133515291322 27.778503481462373, -97.56133509248168 27.778521532079314)))</t>
-        </is>
+        <v>42.94112385639288</v>
       </c>
     </row>
     <row r="33">
@@ -1454,12 +1294,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56126152404838 27.77852133721854, -97.56119911772387 27.778521171892148, -97.56119917817786 27.778503121276103, -97.56126158449209 27.77850328660209, -97.56126152404838 27.77852133721854)))</t>
-        </is>
+        <v>48.57542918650685</v>
       </c>
     </row>
     <row r="34">
@@ -1485,12 +1320,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56118694088023 27.778521139630044, -97.56112453455759 27.778520974269956, -97.56112459502388 27.778502923654422, -97.56118700133626 27.77850308901409, -97.56118694088023 27.778521139630044)))</t>
-        </is>
+        <v>50.72431493096373</v>
       </c>
     </row>
     <row r="35">
@@ -1516,12 +1346,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.5611123546909 27.77852184453206, -97.56104994836952 27.778521679138272, -97.56105000884816 27.778503628523225, -97.56111241515923 27.77850379391661, -97.5611123546909 27.77852184453206)))</t>
-        </is>
+        <v>42.61042088555634</v>
       </c>
     </row>
     <row r="36">
@@ -1547,12 +1372,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56103726415806 27.77852164551821, -97.56097485783854 27.778521480090514, -97.56097491832958 27.77850342947596, -97.56103732463878 27.778503594903245, -97.56103726415806 27.77852164551821)))</t>
-        </is>
+        <v>35.44004687602678</v>
       </c>
     </row>
     <row r="37">
@@ -1578,12 +1398,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>MULTIPOLYGON (((-97.56096471198198 27.778521001923654, -97.5609023056645 27.77852083646322, -97.56090236616754 27.778502785849152, -97.56096477247468 27.778502951309186, -97.56096471198198 27.778521001923654)))</t>
-        </is>
+        <v>24.77106435711227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>